<commit_message>
updates to reading notes
</commit_message>
<xml_diff>
--- a/DataSources_List_Mar23.xlsx
+++ b/DataSources_List_Mar23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cad59077e4daaa4a/Documents/CASA MSc Dissertation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Documents\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{7C98F4DE-0D53-41BB-BA34-C0EE054351BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DC53F0-786A-4FA6-8EE6-5370AA7EF334}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59398AE-B428-4FB2-83CD-B32135C10F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{06033480-126F-48B6-9223-ABB3FB9EF0ED}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{06033480-126F-48B6-9223-ABB3FB9EF0ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>India administrative boundaries</t>
   </si>
   <si>
-    <t>DIVA-GIS</t>
-  </si>
-  <si>
     <t>Objective is to develop a free, and simple but versatile GIS program, that is particularly useful for studying the distribution of biodiversity.</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>TBC</t>
+  </si>
+  <si>
+    <t>GDAL</t>
   </si>
 </sst>
 </file>
@@ -666,12 +666,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="4" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -682,6 +676,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -703,10 +703,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1008,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C800C4-05A4-4CDD-94F4-7D6B4EF4DBCC}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1023,13 +1019,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1226,13 +1222,13 @@
         <v>35</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1246,7 @@
     <hyperlink ref="C12" r:id="rId8" xr:uid="{C31108F7-7824-4D22-8082-D96EED0CFA05}"/>
     <hyperlink ref="C7" r:id="rId9" xr:uid="{939A3353-52C8-412A-980E-716C60AA1496}"/>
     <hyperlink ref="C6" r:id="rId10" xr:uid="{02842A31-18E6-4783-8818-0321FC754F87}"/>
-    <hyperlink ref="C13" r:id="rId11" xr:uid="{6493654D-979A-4516-9D0B-17E66A5C5518}"/>
+    <hyperlink ref="C13" r:id="rId11" display="DIVA-GIS" xr:uid="{6493654D-979A-4516-9D0B-17E66A5C5518}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -1274,185 +1270,185 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1466,7 +1462,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B12" sqref="A10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1478,34 +1474,34 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
@@ -1515,271 +1511,271 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="15"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1791,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DB8095-15A9-4AA0-9384-2749BC4CD7AF}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1804,235 +1800,235 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>68</v>
+        <v>95</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>68</v>
+        <v>55</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>68</v>
+        <v>40</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>68</v>
+        <v>129</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>68</v>
+        <v>130</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>68</v>
+        <v>131</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>69</v>
+        <v>96</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>70</v>
+        <v>121</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>70</v>
+        <v>122</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>70</v>
+        <v>123</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>70</v>
+        <v>124</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>70</v>
+        <v>125</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>70</v>
+        <v>126</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>70</v>
+        <v>127</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>70</v>
+        <v>128</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="D20" s="16"/>
     </row>

</xml_diff>